<commit_message>
fixed grafico de lineas de tendencia
</commit_message>
<xml_diff>
--- a/src/informesGenerados/PextListado.xlsx
+++ b/src/informesGenerados/PextListado.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
   <si>
     <t>Unidad Organizativa</t>
   </si>
@@ -49,190 +49,280 @@
     <t>CDNT</t>
   </si>
   <si>
-    <t>DTHO</t>
-  </si>
-  <si>
-    <t>2019-05-02</t>
-  </si>
-  <si>
-    <t>Afectación a la planta exterior por  corte  y sustracción de FO Carretera Naranjo Agrio-Alcarraza, entre 4 Caminos y Zarza Arriba</t>
-  </si>
-  <si>
-    <t>Sagua de Tánamo</t>
-  </si>
-  <si>
-    <t>7436/19</t>
+    <t>DTSR</t>
+  </si>
+  <si>
+    <t>2020-02-03</t>
+  </si>
+  <si>
+    <t>Afectación a la planta exterior por  corte y sustracción de unbajante telefónico Calle San José</t>
+  </si>
+  <si>
+    <t>Arroyo Naranjo</t>
+  </si>
+  <si>
+    <t>6877/20</t>
+  </si>
+  <si>
+    <t>Bajante telefónico</t>
+  </si>
+  <si>
+    <t>DVLH-02-20-0022</t>
+  </si>
+  <si>
+    <t>Afectación a la planta exterior por  corte de un cable telefónico de 50 pares Calle Silvia  y Concordia</t>
+  </si>
+  <si>
+    <t>Cable telefónico</t>
+  </si>
+  <si>
+    <t>DVLH-02-20-0023</t>
+  </si>
+  <si>
+    <t>DTSC</t>
+  </si>
+  <si>
+    <t>2020-02-04</t>
+  </si>
+  <si>
+    <t>Afectación a la planta exterior por  corte y sustracción de unbajante telefónico Entrada de Dos Caminos. Lateral de la UBPC</t>
+  </si>
+  <si>
+    <t>San Luis (SC)</t>
+  </si>
+  <si>
+    <t>2047/20</t>
+  </si>
+  <si>
+    <t>DTSC-02-20-0015</t>
+  </si>
+  <si>
+    <t>2020-02-05</t>
+  </si>
+  <si>
+    <t>Afectación a la planta exterior por  corte de un cable telefónico de 100 pares Calle Morris, entre Pasaje A y José Miguel</t>
+  </si>
+  <si>
+    <t>7188/20</t>
+  </si>
+  <si>
+    <t>DVLH-02-20-0024</t>
+  </si>
+  <si>
+    <t>DTCM</t>
+  </si>
+  <si>
+    <t>2020-02-07</t>
+  </si>
+  <si>
+    <t>Afectación a la planta exterior por  corte y sustracción de FO (aérea) Carretera Camagüey Minas</t>
+  </si>
+  <si>
+    <t>Camagüey</t>
+  </si>
+  <si>
+    <t>13/20</t>
   </si>
   <si>
     <t>Fibra óptica</t>
   </si>
   <si>
-    <t>DTHO-05-19-0033</t>
-  </si>
-  <si>
-    <t>DTSC</t>
-  </si>
-  <si>
-    <t>2019-05-09</t>
-  </si>
-  <si>
-    <t>Afectación a la planta exterior por  corte  y sustracción de cable de cobre Localidad Guaranal. Contramaestre</t>
-  </si>
-  <si>
-    <t>Contramaestre</t>
-  </si>
-  <si>
-    <t>6935/19</t>
-  </si>
-  <si>
-    <t>Alambre de cobre</t>
-  </si>
-  <si>
-    <t>DTSC-05-19-0033</t>
-  </si>
-  <si>
-    <t>DTAR</t>
-  </si>
-  <si>
-    <t>2019-05-13</t>
-  </si>
-  <si>
-    <t>Afectación a la planta exterior por  corte  de FO Carretera Bahía Honda Cabañas</t>
-  </si>
-  <si>
-    <t>Bahía Honda</t>
-  </si>
-  <si>
-    <t>3880/19</t>
-  </si>
-  <si>
-    <t>DTAR-05-19-0052</t>
-  </si>
-  <si>
-    <t>Afectación a la planta exterior por  corte  y sustracción bajante telefónico Mariana de la Torre</t>
-  </si>
-  <si>
-    <t>Holguín</t>
-  </si>
-  <si>
-    <t>8189/19</t>
-  </si>
-  <si>
-    <t>Bajante telefónico</t>
-  </si>
-  <si>
-    <t>DTHO-05-19-0037</t>
-  </si>
-  <si>
-    <t>2019-05-14</t>
-  </si>
-  <si>
-    <t>Afectación a la planta exterior por  corte  y sustracción de bitubo de FO Carretera a San Germán</t>
-  </si>
-  <si>
-    <t>Urbano Noris</t>
-  </si>
-  <si>
-    <t>8156/19</t>
-  </si>
-  <si>
-    <t>DTHO-05-19-0038</t>
-  </si>
-  <si>
-    <t>2019-05-15</t>
-  </si>
-  <si>
-    <t>Afectación a la planta exterior por  corte  y sustracción de cable tensor Carretera San Germán a 1 Km del vertedero</t>
-  </si>
-  <si>
-    <t>8126/19</t>
+    <t>DTCM-02-20-0012</t>
+  </si>
+  <si>
+    <t>2020-02-10</t>
+  </si>
+  <si>
+    <t>Afectación a la planta exterior por  corte de un cable aéreo de 100 pares, por segunda ocación Calle Silvia, entre Concordia y San Agustín</t>
+  </si>
+  <si>
+    <t>8249/20</t>
+  </si>
+  <si>
+    <t>DVLH-02-20-0028</t>
+  </si>
+  <si>
+    <t>Afectación a la planta exterior por  corte de 2 cables aeréos de 30 y 100 pares respectivamente Calle Morris y Pasaje B</t>
+  </si>
+  <si>
+    <t>DVLH-02-20-0029</t>
+  </si>
+  <si>
+    <t>DTSS</t>
+  </si>
+  <si>
+    <t>2020-02-11</t>
+  </si>
+  <si>
+    <t>Afectación a la planta exterior por  sustracción de 2 tapas de registros Localidad de Topes de Collantes</t>
+  </si>
+  <si>
+    <t>Trinidad</t>
+  </si>
+  <si>
+    <t>1460/20</t>
+  </si>
+  <si>
+    <t>Tensor de anclaje</t>
+  </si>
+  <si>
+    <t>DTSS-02-20-0029</t>
+  </si>
+  <si>
+    <t>DTMZ</t>
+  </si>
+  <si>
+    <t>2020-02-13</t>
+  </si>
+  <si>
+    <t>Afectación a la planta exterior por  corte y sustracción de tensor Carretera San Miguel de los Baños a Coliseo</t>
+  </si>
+  <si>
+    <t>Jovellanos</t>
+  </si>
+  <si>
+    <t>2067/20</t>
   </si>
   <si>
     <t>Tensor</t>
   </si>
   <si>
-    <t>DTHO-05-19-0039</t>
+    <t>DTMZ-02-20-0016</t>
+  </si>
+  <si>
+    <t>2020-02-14</t>
+  </si>
+  <si>
+    <t>Afectación a la planta exterior por  corte de cable aéreo de 400 pares Cale José Miguel, entre Pasaje D y Concordia</t>
+  </si>
+  <si>
+    <t>9099/20</t>
+  </si>
+  <si>
+    <t>DVLH-02-20-0032</t>
+  </si>
+  <si>
+    <t>Afectación a la planta exterior por  corte de cable aéreo de 50 pares Calle Rosell, entre Mendoza y Arellano</t>
+  </si>
+  <si>
+    <t>DVLH-02-20-0033</t>
   </si>
   <si>
     <t>DTGR</t>
   </si>
   <si>
-    <t>2019-05-28</t>
-  </si>
-  <si>
-    <t>Afectación a la planta exterior por  corte  y sustracción de Bajante telefónico Calle Manuel de Socorro No. 730,  entre Mariana Grajales y Roberto Reyes</t>
+    <t>2020-02-16</t>
+  </si>
+  <si>
+    <t>Afectación a la planta exterior por  corte y sustracción de bajante telefónico Calle 46, entre 26 de Julio y 19</t>
   </si>
   <si>
     <t>Bayamo</t>
   </si>
   <si>
-    <t>5877/19</t>
-  </si>
-  <si>
-    <t>DTGR-05-19-0051</t>
-  </si>
-  <si>
-    <t>2019-05-29</t>
-  </si>
-  <si>
-    <t>Afectación a la planta exterior por  corte  y sustracción de Bajante telefónico Calle 26 de Julio, entre 2da y Osvaldo Lara</t>
-  </si>
-  <si>
-    <t>5903/19</t>
-  </si>
-  <si>
-    <t>DTGR-05-19-0052</t>
-  </si>
-  <si>
-    <t>DTVC</t>
-  </si>
-  <si>
-    <t>Afectación a la planta exterior por  corte  de FO aérea Ave. Ismaelillo y Callejón de Los Caneyes</t>
-  </si>
-  <si>
-    <t>Santa Clara</t>
-  </si>
-  <si>
-    <t>5574/19</t>
-  </si>
-  <si>
-    <t>DTVC-05-19-0113</t>
-  </si>
-  <si>
-    <t>DTSR</t>
-  </si>
-  <si>
-    <t>2019-05-30</t>
-  </si>
-  <si>
-    <t>Afectación a la planta exterior por  corte  y sustracción de Bajante telefónico Carretera Santa Maria del Rosario y 8 Vías</t>
-  </si>
-  <si>
-    <t>Cotorro</t>
-  </si>
-  <si>
-    <t>35381/19</t>
-  </si>
-  <si>
-    <t>DVLH-05-19-0117</t>
-  </si>
-  <si>
-    <t>2019-05-31</t>
-  </si>
-  <si>
-    <t>Afectación a la planta exterior por  corte de cable autosoportado de 50 pares Km 4 1/2. Carretera de Mar Verde</t>
-  </si>
-  <si>
-    <t>Santiago de Cuba</t>
-  </si>
-  <si>
-    <t>8098/19</t>
-  </si>
-  <si>
-    <t>Cable telefónico</t>
-  </si>
-  <si>
-    <t>DTSC-05-19-0041</t>
+    <t>2029/20</t>
+  </si>
+  <si>
+    <t>DTGR-02-20-0018</t>
+  </si>
+  <si>
+    <t>2020-02-18</t>
+  </si>
+  <si>
+    <t>Afectación a la planta exterior por  corte de FO Calle Isabel, entre Sofia y Estela</t>
+  </si>
+  <si>
+    <t>10020/20</t>
+  </si>
+  <si>
+    <t>DVLH-02-20-0039</t>
+  </si>
+  <si>
+    <t>2020-02-27</t>
+  </si>
+  <si>
+    <t>Afectación a la planta exterior por  corte y sustracción de bajante telefónico Calle Cisnero No . 411,  entre Camilo Cienfuegos y 1ra</t>
+  </si>
+  <si>
+    <t>Palma Soriano</t>
+  </si>
+  <si>
+    <t>3139/20</t>
+  </si>
+  <si>
+    <t>DTSC-02-20-0022</t>
+  </si>
+  <si>
+    <t>2020-02-22</t>
+  </si>
+  <si>
+    <t>Afectación a la planta exterior por   sustracción de 2 AP (wifi) Calle 9, entre 3ra y Avenida Granma</t>
+  </si>
+  <si>
+    <t>2290/20</t>
+  </si>
+  <si>
+    <t>Cable simétrico</t>
+  </si>
+  <si>
+    <t>DTGR-02-20-0026</t>
+  </si>
+  <si>
+    <t>Afectación a la planta exterior por  sustracción de AP (wifi) Calle 11</t>
+  </si>
+  <si>
+    <t>DTGR-02-20-0027</t>
+  </si>
+  <si>
+    <t>Afectación a la planta exterior por  corte  de 5 cables multipar Calle Victoria, entre San Agustín y Unión</t>
+  </si>
+  <si>
+    <t>10947/20</t>
+  </si>
+  <si>
+    <t>DVLH-02-20-0045</t>
+  </si>
+  <si>
+    <t>DTMY</t>
+  </si>
+  <si>
+    <t>2020-02-25</t>
+  </si>
+  <si>
+    <t>Afectación a la planta exterior por  corte y sustracción de alambre de coser Carretera de San Felipe</t>
+  </si>
+  <si>
+    <t>Quivicán</t>
+  </si>
+  <si>
+    <t>1330/20</t>
+  </si>
+  <si>
+    <t>Alambre de coser</t>
+  </si>
+  <si>
+    <t>DTMY-02-20-0012</t>
+  </si>
+  <si>
+    <t>Afectación a la planta exterior por corte a 4 cables multipar(2 de 400 pares y 2 de 200 pares) Calle 100 y Autopista Oeste.</t>
+  </si>
+  <si>
+    <t>11603</t>
+  </si>
+  <si>
+    <t>DVLH-02-20-0048</t>
+  </si>
+  <si>
+    <t>2020-02-28</t>
+  </si>
+  <si>
+    <t>Afectación a la planta exterior por corte y sustracción de  alambre spring Ruta La Carlota la Mulata</t>
+  </si>
+  <si>
+    <t>2719/20</t>
+  </si>
+  <si>
+    <t>DTMZ-02-20-0020</t>
   </si>
 </sst>
 </file>
@@ -690,7 +780,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
   <sheetPr/>
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1" zoomScaleNormal="100" zoomScaleSheetLayoutView="60" zoomScale="100" view="normal"/>
   </sheetViews>
@@ -759,19 +849,19 @@
         <v>15</v>
       </c>
       <c r="F2" s="3">
-        <v>260.4</v>
+        <v>0</v>
       </c>
       <c r="G2" s="3">
-        <v>359.68</v>
+        <v>0</v>
       </c>
       <c r="H2" s="3">
-        <v>196</v>
+        <v>8</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>16</v>
       </c>
       <c r="J2" s="3">
-        <v>1</v>
+        <v>400</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>17</v>
@@ -779,72 +869,72 @@
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="D3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0</v>
+      </c>
+      <c r="H3" s="3">
+        <v>8</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="J3" s="3">
+        <v>50</v>
+      </c>
+      <c r="K3" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="3">
-        <v>7320.96</v>
-      </c>
-      <c r="G3" s="3">
-        <v>375.1</v>
-      </c>
-      <c r="H3" s="3">
-        <v>2</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="3">
-        <v>60</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="F4" s="3">
-        <v>17.16</v>
+        <v>45.56</v>
       </c>
       <c r="G4" s="3">
-        <v>294.63</v>
+        <v>56.92</v>
       </c>
       <c r="H4" s="3">
-        <v>238</v>
+        <v>3</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>16</v>
       </c>
       <c r="J4" s="3">
-        <v>1</v>
+        <v>130</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5">
@@ -852,69 +942,69 @@
         <v>11</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F5" s="3">
-        <v>18.75</v>
+        <v>249</v>
       </c>
       <c r="G5" s="3">
-        <v>0</v>
+        <v>1466.85</v>
       </c>
       <c r="H5" s="3">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="J5" s="3">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="3">
+        <v>226.7</v>
+      </c>
+      <c r="G6" s="3">
+        <v>6174.55</v>
+      </c>
+      <c r="H6" s="3">
+        <v>140</v>
+      </c>
+      <c r="I6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="J6" s="3">
+        <v>19</v>
+      </c>
+      <c r="K6" s="5" t="s">
         <v>37</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F6" s="3">
-        <v>3.25</v>
-      </c>
-      <c r="G6" s="3">
-        <v>0</v>
-      </c>
-      <c r="H6" s="3">
-        <v>0</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J6" s="3">
-        <v>13</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="7">
@@ -922,209 +1012,524 @@
         <v>11</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0</v>
+      </c>
+      <c r="H7" s="3">
+        <v>15</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" s="3">
+        <v>60</v>
+      </c>
+      <c r="K7" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F7" s="3">
-        <v>0</v>
-      </c>
-      <c r="G7" s="3">
-        <v>0</v>
-      </c>
-      <c r="H7" s="3">
-        <v>0</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="J7" s="3">
-        <v>50</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>46</v>
+        <v>11</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F8" s="3">
-        <v>6.04</v>
+        <v>0</v>
       </c>
       <c r="G8" s="3">
-        <v>4.95</v>
+        <v>0</v>
       </c>
       <c r="H8" s="3">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="J8" s="3">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>53</v>
-      </c>
       <c r="D9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="F9" s="3">
-        <v>59.12</v>
-      </c>
-      <c r="G9" s="3">
-        <v>57.42</v>
-      </c>
-      <c r="H9" s="3">
-        <v>5</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="J9" s="3">
-        <v>350</v>
+        <v>2</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>52</v>
       </c>
       <c r="C10" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0</v>
+      </c>
+      <c r="H10" s="3">
+        <v>2</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="J10" s="3">
+        <v>250</v>
+      </c>
+      <c r="K10" s="5" t="s">
         <v>57</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F10" s="3">
-        <v>570.32</v>
-      </c>
-      <c r="G10" s="3">
-        <v>166.82</v>
-      </c>
-      <c r="H10" s="3">
-        <v>1</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J10" s="3">
-        <v>1</v>
-      </c>
-      <c r="K10" s="5" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F11" s="3">
-        <v>18.72</v>
+        <v>1917.6</v>
       </c>
       <c r="G11" s="3">
-        <v>149.41</v>
+        <v>22313.7</v>
       </c>
       <c r="H11" s="3">
-        <v>1</v>
+        <v>400</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="J11" s="3">
         <v>60</v>
       </c>
       <c r="K11" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0</v>
+      </c>
+      <c r="H12" s="3">
+        <v>50</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J12" s="3">
+        <v>140</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="6" t="s">
+      <c r="D13" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="E13" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="F13" s="3">
+        <v>17.05</v>
+      </c>
+      <c r="G13" s="3">
+        <v>9.08</v>
+      </c>
+      <c r="H13" s="3">
+        <v>1</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J13" s="3">
+        <v>50</v>
+      </c>
+      <c r="K13" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="E12" s="6" t="s">
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F12" s="6">
+      <c r="C14" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J14" s="3">
+        <v>600</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F15" s="3">
+        <v>14</v>
+      </c>
+      <c r="G15" s="3">
+        <v>36.76</v>
+      </c>
+      <c r="H15" s="3">
+        <v>1</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J15" s="3">
+        <v>25</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F16" s="3">
+        <v>1520.82</v>
+      </c>
+      <c r="G16" s="3">
+        <v>0</v>
+      </c>
+      <c r="H16" s="3">
+        <v>0</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="J16" s="3">
+        <v>2</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F17" s="3">
+        <v>512.83</v>
+      </c>
+      <c r="G17" s="3">
+        <v>0</v>
+      </c>
+      <c r="H17" s="3">
+        <v>0</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="J17" s="3">
+        <v>1</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F18" s="3">
+        <v>1484</v>
+      </c>
+      <c r="G18" s="3">
+        <v>16800</v>
+      </c>
+      <c r="H18" s="3">
+        <v>350</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J18" s="3">
+        <v>5</v>
+      </c>
+      <c r="K18" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0</v>
+      </c>
+      <c r="G19" s="3">
+        <v>0</v>
+      </c>
+      <c r="H19" s="3">
+        <v>0</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="J19" s="3">
+        <v>300</v>
+      </c>
+      <c r="K19" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="G12" s="6">
-        <v>129.79</v>
-      </c>
-      <c r="H12" s="6">
-        <v>0</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="J12" s="6">
-        <v>40</v>
-      </c>
-      <c r="K12" s="8" t="s">
-        <v>72</v>
+      <c r="D20" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F20" s="3">
+        <v>826.64</v>
+      </c>
+      <c r="G20" s="3">
+        <v>3807.6</v>
+      </c>
+      <c r="H20" s="3">
+        <v>62</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J20" s="3">
+        <v>4</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="F21" s="6">
+        <v>0</v>
+      </c>
+      <c r="G21" s="6">
+        <v>0</v>
+      </c>
+      <c r="H21" s="6">
+        <v>4</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="J21" s="6">
+        <v>150</v>
+      </c>
+      <c r="K21" s="8" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>